<commit_message>
classifications and properties creator done
</commit_message>
<xml_diff>
--- a/server/test/csv-files/molecules.xlsx
+++ b/server/test/csv-files/molecules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\csv-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC401603-8394-48D8-90BD-FA5274E70476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F80D6A-8F07-4F40-A0DE-138CBA367822}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1360,11 +1360,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,7 +1809,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>80</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>81</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>87</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>88</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>89</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>86</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>99</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>101</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>103</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>105</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>107</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>130</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>131</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>132</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>133</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>134</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>129</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>140</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>141</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>142</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>143</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
         <v>149</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>150</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>151</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>152</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>153</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>154</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>155</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>148</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>158</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>160</v>
       </c>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="Q100" s="23"/>
     </row>
-    <row r="101" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>159</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>162</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>163</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>166</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>169</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>168</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>171</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>174</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>175</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>172</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>176</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>177</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>178</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>173</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>182</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>183</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>186</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>185</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="28.8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
         <v>190</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="28.8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>191</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="28.8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
         <v>192</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>217</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>218</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>219</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>220</v>
       </c>

</xml_diff>